<commit_message>
adding versions to CAD Folders
</commit_message>
<xml_diff>
--- a/DOCS/KC_BOM.xlsx
+++ b/DOCS/KC_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tier3tech-my.sharepoint.com/personal/kevin_badgepirates_com/Documents/Badges/BSidesKC23/DOCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6FC27E1A-1A92-4826-A887-D3236D885D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035721DD-278C-4843-B924-45D9B85DE0FE}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{6FC27E1A-1A92-4826-A887-D3236D885D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EF740EE-E191-4A1E-BB21-C0FAEE6EF781}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57810" windowHeight="28605" xr2:uid="{062BDCAA-2B8B-4A5F-A04B-1DCDD0935ACE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="40305" windowHeight="17475" xr2:uid="{062BDCAA-2B8B-4A5F-A04B-1DCDD0935ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="OzSec Badge + Detail (Paths)" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="162">
   <si>
     <t>Id</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Supplier and ref</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>_1</t>
   </si>
   <si>
@@ -515,6 +512,27 @@
   </si>
   <si>
     <t>D10</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Reel - 700</t>
+  </si>
+  <si>
+    <t>Reel - 5000</t>
+  </si>
+  <si>
+    <t>Reel - 4000</t>
+  </si>
+  <si>
+    <t>Reel - 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reel - 500 </t>
+  </si>
+  <si>
+    <t>Reel - 3000</t>
   </si>
 </sst>
 </file>
@@ -602,7 +620,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -684,7 +702,7 @@
     <tableColumn id="4" xr3:uid="{FAADF724-2F4A-44A3-8B51-241720D073A5}" uniqueName="4" name="Quantity" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{B75F10CD-E16B-470A-B3F7-2BEB5548300E}" uniqueName="5" name="Designation" queryTableFieldId="5" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{4027EEF2-8F57-4736-B6DC-4EF6405FDCD1}" uniqueName="6" name="Supplier and ref" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{97B3ADF6-DF4A-4CDB-A56A-8360BE27790A}" uniqueName="7" name="Column1" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{97B3ADF6-DF4A-4CDB-A56A-8360BE27790A}" uniqueName="7" name="Stock" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -990,7 +1008,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,10 +1029,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1032,7 +1050,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1040,25 +1058,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1066,25 +1084,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1092,25 +1110,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
       <c r="F4">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1118,28 +1136,28 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4">
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1147,28 +1165,28 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1176,25 +1194,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>19</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1202,25 +1220,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1228,25 +1246,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1254,25 +1272,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>25</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1280,28 +1298,28 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,28 +1327,28 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
         <v>45</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1338,28 +1356,28 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1367,28 +1385,28 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>124</v>
       </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>125</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1396,28 +1414,28 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>32</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
       <c r="H15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1425,28 +1443,28 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>114</v>
       </c>
-      <c r="D16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>115</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1454,28 +1472,28 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1483,28 +1501,28 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>6</v>
       </c>
       <c r="G18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1512,28 +1530,28 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
         <v>35</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>36</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1541,28 +1559,28 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>57</v>
       </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>58</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1570,28 +1588,28 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>82</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>83</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1599,25 +1617,25 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" t="s">
         <v>153</v>
       </c>
-      <c r="D22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" t="s">
-        <v>154</v>
-      </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1625,28 +1643,28 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1654,28 +1672,28 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1683,28 +1701,28 @@
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1712,28 +1730,28 @@
         <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1741,28 +1759,28 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1770,28 +1788,28 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1799,28 +1817,28 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1828,28 +1846,28 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1857,28 +1875,28 @@
         <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
         <v>55</v>
       </c>
-      <c r="E31" t="s">
-        <v>56</v>
-      </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1886,28 +1904,28 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
         <v>47</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
         <v>48</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>49</v>
-      </c>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1915,28 +1933,28 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1944,28 +1962,28 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
         <v>69</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>70</v>
-      </c>
       <c r="H34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I34" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1973,28 +1991,28 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
         <v>103</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
         <v>53</v>
       </c>
-      <c r="E35" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
       <c r="H35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2002,28 +2020,28 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
         <v>103</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
         <v>37</v>
       </c>
-      <c r="E36" t="s">
-        <v>104</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
-        <v>38</v>
-      </c>
       <c r="H36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2031,28 +2049,28 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
         <v>30</v>
       </c>
-      <c r="E37" t="s">
-        <v>104</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>31</v>
-      </c>
       <c r="H37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2060,28 +2078,28 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
         <v>103</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
         <v>39</v>
       </c>
-      <c r="E38" t="s">
-        <v>104</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38" t="s">
-        <v>40</v>
-      </c>
       <c r="H38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2089,28 +2107,28 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" t="s">
         <v>103</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
         <v>41</v>
       </c>
-      <c r="E39" t="s">
-        <v>104</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>42</v>
-      </c>
       <c r="H39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2118,28 +2136,28 @@
         <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
         <v>65</v>
       </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>66</v>
-      </c>
       <c r="H40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2147,28 +2165,28 @@
         <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" t="s">
         <v>62</v>
       </c>
-      <c r="E41" t="s">
-        <v>63</v>
-      </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2176,28 +2194,25 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" t="s">
         <v>134</v>
-      </c>
-      <c r="D42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" t="s">
-        <v>134</v>
-      </c>
-      <c r="H42" t="s">
-        <v>135</v>
-      </c>
-      <c r="I42" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2205,36 +2220,36 @@
         <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
+        <v>150</v>
+      </c>
+      <c r="F45" t="s">
         <v>151</v>
-      </c>
-      <c r="F45" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>